<commit_message>
Re #1 minor changes to  V4 building WorkPlan
</commit_message>
<xml_diff>
--- a/documentation/design_forV4/WorkPlan.xlsx
+++ b/documentation/design_forV4/WorkPlan.xlsx
@@ -9,13 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="0" windowWidth="21750" windowHeight="10170"/>
+    <workbookView xWindow="2790" yWindow="0" windowWidth="21750" windowHeight="10170"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
   <si>
     <t>W1</t>
   </si>
@@ -72,9 +71,6 @@
     <t>compiled Horace</t>
   </si>
   <si>
-    <t>MPI frmwk investigation</t>
-  </si>
-  <si>
     <t>extracting projection interface</t>
   </si>
   <si>
@@ -90,10 +86,16 @@
     <t>Parallel cut</t>
   </si>
   <si>
-    <t>parallel unit operations/sqw eval</t>
-  </si>
-  <si>
     <t>q-dE projection</t>
+  </si>
+  <si>
+    <t>C++ MPI frmwk investigation</t>
+  </si>
+  <si>
+    <t>Parallel sqw eval</t>
+  </si>
+  <si>
+    <t>parallel unit operations</t>
   </si>
 </sst>
 </file>
@@ -116,7 +118,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -153,6 +155,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="20">
     <border>
@@ -379,7 +387,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -410,6 +418,27 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -419,15 +448,6 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -437,16 +457,13 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -736,10 +753,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L21"/>
+  <dimension ref="A1:L25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:M21"/>
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -798,7 +815,7 @@
     </row>
     <row r="3" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="9"/>
@@ -859,12 +876,12 @@
       <c r="L6" s="6"/>
     </row>
     <row r="7" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="35" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" s="28"/>
-      <c r="C7" s="28"/>
-      <c r="D7" s="28"/>
+      <c r="A7" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="25"/>
+      <c r="C7" s="25"/>
+      <c r="D7" s="25"/>
       <c r="E7" s="3"/>
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
@@ -879,12 +896,12 @@
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
-      <c r="E8" s="27" t="s">
-        <v>16</v>
-      </c>
-      <c r="F8" s="28"/>
-      <c r="G8" s="28"/>
-      <c r="H8" s="28"/>
+      <c r="E8" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" s="25"/>
+      <c r="G8" s="25"/>
+      <c r="H8" s="25"/>
       <c r="I8" s="10"/>
       <c r="J8" s="4"/>
       <c r="K8" s="4"/>
@@ -899,12 +916,12 @@
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>
-      <c r="I9" s="27" t="s">
+      <c r="I9" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="J9" s="28"/>
-      <c r="K9" s="28"/>
-      <c r="L9" s="29"/>
+      <c r="J9" s="25"/>
+      <c r="K9" s="25"/>
+      <c r="L9" s="27"/>
     </row>
     <row r="10" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5"/>
@@ -929,12 +946,12 @@
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
-      <c r="I11" s="27" t="s">
-        <v>18</v>
-      </c>
-      <c r="J11" s="28"/>
-      <c r="K11" s="28"/>
-      <c r="L11" s="29"/>
+      <c r="I11" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="J11" s="25"/>
+      <c r="K11" s="25"/>
+      <c r="L11" s="27"/>
     </row>
     <row r="12" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5"/>
@@ -959,12 +976,12 @@
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
-      <c r="I13" s="27" t="s">
-        <v>19</v>
-      </c>
-      <c r="J13" s="28"/>
-      <c r="K13" s="28"/>
-      <c r="L13" s="29"/>
+      <c r="I13" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="J13" s="25"/>
+      <c r="K13" s="25"/>
+      <c r="L13" s="27"/>
     </row>
     <row r="14" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="5"/>
@@ -989,12 +1006,12 @@
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
-      <c r="I15" s="27" t="s">
-        <v>22</v>
-      </c>
-      <c r="J15" s="28"/>
-      <c r="K15" s="28"/>
-      <c r="L15" s="29"/>
+      <c r="I15" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="J15" s="25"/>
+      <c r="K15" s="25"/>
+      <c r="L15" s="27"/>
     </row>
     <row r="16" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="5"/>
@@ -1019,12 +1036,12 @@
       <c r="F17" s="4"/>
       <c r="G17" s="4"/>
       <c r="H17" s="4"/>
-      <c r="I17" s="24" t="s">
+      <c r="I17" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="J17" s="25"/>
-      <c r="K17" s="25"/>
-      <c r="L17" s="26"/>
+      <c r="J17" s="32"/>
+      <c r="K17" s="32"/>
+      <c r="L17" s="33"/>
     </row>
     <row r="18" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="5"/>
@@ -1049,11 +1066,11 @@
       <c r="F19" s="4"/>
       <c r="G19" s="4"/>
       <c r="H19" s="4"/>
-      <c r="I19" s="36" t="s">
-        <v>20</v>
-      </c>
-      <c r="J19" s="33"/>
-      <c r="K19" s="34"/>
+      <c r="I19" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="J19" s="29"/>
+      <c r="K19" s="30"/>
       <c r="L19" s="6"/>
     </row>
     <row r="20" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1071,23 +1088,88 @@
       <c r="L20" s="6"/>
     </row>
     <row r="21" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="7"/>
-      <c r="B21" s="8"/>
-      <c r="C21" s="8"/>
-      <c r="D21" s="8"/>
-      <c r="E21" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="F21" s="31"/>
-      <c r="G21" s="31"/>
-      <c r="H21" s="31"/>
-      <c r="I21" s="32"/>
-      <c r="J21" s="8"/>
-      <c r="K21" s="8"/>
-      <c r="L21" s="12"/>
+      <c r="A21" s="5"/>
+      <c r="B21" s="4"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="34" t="s">
+        <v>23</v>
+      </c>
+      <c r="F21" s="35"/>
+      <c r="G21" s="35"/>
+      <c r="H21" s="35"/>
+      <c r="I21" s="36"/>
+      <c r="J21" s="4"/>
+      <c r="K21" s="4"/>
+      <c r="L21" s="6"/>
+    </row>
+    <row r="22" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="5"/>
+      <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="15"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="4"/>
+      <c r="H22" s="4"/>
+      <c r="I22" s="4"/>
+      <c r="J22" s="4"/>
+      <c r="K22" s="4"/>
+      <c r="L22" s="6"/>
+    </row>
+    <row r="23" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="5"/>
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="37" t="s">
+        <v>19</v>
+      </c>
+      <c r="F23" s="38"/>
+      <c r="G23" s="39"/>
+      <c r="H23" s="4"/>
+      <c r="I23" s="4"/>
+      <c r="J23" s="4"/>
+      <c r="K23" s="4"/>
+      <c r="L23" s="6"/>
+    </row>
+    <row r="24" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="5"/>
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="15"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="4"/>
+      <c r="H24" s="4"/>
+      <c r="I24" s="4"/>
+      <c r="J24" s="4"/>
+      <c r="K24" s="4"/>
+      <c r="L24" s="6"/>
+    </row>
+    <row r="25" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="7"/>
+      <c r="B25" s="8"/>
+      <c r="C25" s="8"/>
+      <c r="D25" s="8"/>
+      <c r="E25" s="37" t="s">
+        <v>22</v>
+      </c>
+      <c r="F25" s="38"/>
+      <c r="G25" s="39"/>
+      <c r="H25" s="8"/>
+      <c r="I25" s="8"/>
+      <c r="J25" s="8"/>
+      <c r="K25" s="8"/>
+      <c r="L25" s="12"/>
     </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="13">
+    <mergeCell ref="E21:I21"/>
+    <mergeCell ref="I9:L9"/>
+    <mergeCell ref="I13:L13"/>
+    <mergeCell ref="E23:G23"/>
+    <mergeCell ref="E25:G25"/>
     <mergeCell ref="D4:I4"/>
     <mergeCell ref="A7:D7"/>
     <mergeCell ref="E8:H8"/>
@@ -1096,9 +1178,6 @@
     <mergeCell ref="J5:L5"/>
     <mergeCell ref="I17:L17"/>
     <mergeCell ref="I11:L11"/>
-    <mergeCell ref="E21:I21"/>
-    <mergeCell ref="I9:L9"/>
-    <mergeCell ref="I13:L13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Re #1 Horace 08/11/2019 Kick-in meeting presentation
</commit_message>
<xml_diff>
--- a/documentation/design_forV4/WorkPlan.xlsx
+++ b/documentation/design_forV4/WorkPlan.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2790" yWindow="0" windowWidth="21750" windowHeight="10170"/>
+    <workbookView xWindow="3750" yWindow="0" windowWidth="21750" windowHeight="10170"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
   <si>
     <t>W1</t>
   </si>
@@ -96,6 +96,9 @@
   </si>
   <si>
     <t>parallel unit operations</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> HDF file format</t>
   </si>
 </sst>
 </file>
@@ -118,7 +121,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -161,6 +164,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="20">
     <border>
@@ -387,7 +396,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -409,6 +418,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -421,15 +451,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -448,22 +469,11 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -753,10 +763,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L25"/>
+  <dimension ref="A1:L27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -833,14 +843,14 @@
       <c r="A4" s="5"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
-      <c r="D4" s="21" t="s">
+      <c r="D4" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="22"/>
-      <c r="F4" s="22"/>
-      <c r="G4" s="22"/>
-      <c r="H4" s="22"/>
-      <c r="I4" s="23"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="29"/>
+      <c r="G4" s="29"/>
+      <c r="H4" s="29"/>
+      <c r="I4" s="30"/>
       <c r="J4" s="4"/>
       <c r="K4" s="4"/>
       <c r="L4" s="6"/>
@@ -855,11 +865,11 @@
       <c r="G5" s="13"/>
       <c r="H5" s="13"/>
       <c r="I5" s="11"/>
-      <c r="J5" s="21" t="s">
+      <c r="J5" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="K5" s="22"/>
-      <c r="L5" s="23"/>
+      <c r="K5" s="29"/>
+      <c r="L5" s="30"/>
     </row>
     <row r="6" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5"/>
@@ -876,12 +886,12 @@
       <c r="L6" s="6"/>
     </row>
     <row r="7" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="24" t="s">
+      <c r="A7" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="25"/>
-      <c r="C7" s="25"/>
-      <c r="D7" s="25"/>
+      <c r="B7" s="24"/>
+      <c r="C7" s="24"/>
+      <c r="D7" s="24"/>
       <c r="E7" s="3"/>
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
@@ -896,12 +906,12 @@
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
-      <c r="E8" s="26" t="s">
+      <c r="E8" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="F8" s="25"/>
-      <c r="G8" s="25"/>
-      <c r="H8" s="25"/>
+      <c r="F8" s="24"/>
+      <c r="G8" s="24"/>
+      <c r="H8" s="24"/>
       <c r="I8" s="10"/>
       <c r="J8" s="4"/>
       <c r="K8" s="4"/>
@@ -916,12 +926,12 @@
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>
-      <c r="I9" s="26" t="s">
+      <c r="I9" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="J9" s="25"/>
-      <c r="K9" s="25"/>
-      <c r="L9" s="27"/>
+      <c r="J9" s="24"/>
+      <c r="K9" s="24"/>
+      <c r="L9" s="25"/>
     </row>
     <row r="10" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5"/>
@@ -946,12 +956,12 @@
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
-      <c r="I11" s="26" t="s">
+      <c r="I11" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="J11" s="25"/>
-      <c r="K11" s="25"/>
-      <c r="L11" s="27"/>
+      <c r="J11" s="24"/>
+      <c r="K11" s="24"/>
+      <c r="L11" s="25"/>
     </row>
     <row r="12" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5"/>
@@ -976,12 +986,12 @@
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
-      <c r="I13" s="26" t="s">
+      <c r="I13" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="J13" s="25"/>
-      <c r="K13" s="25"/>
-      <c r="L13" s="27"/>
+      <c r="J13" s="24"/>
+      <c r="K13" s="24"/>
+      <c r="L13" s="25"/>
     </row>
     <row r="14" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="5"/>
@@ -1006,12 +1016,12 @@
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
-      <c r="I15" s="26" t="s">
+      <c r="I15" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="J15" s="25"/>
-      <c r="K15" s="25"/>
-      <c r="L15" s="27"/>
+      <c r="J15" s="24"/>
+      <c r="K15" s="24"/>
+      <c r="L15" s="25"/>
     </row>
     <row r="16" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="5"/>
@@ -1036,12 +1046,12 @@
       <c r="F17" s="4"/>
       <c r="G17" s="4"/>
       <c r="H17" s="4"/>
-      <c r="I17" s="31" t="s">
+      <c r="I17" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="J17" s="32"/>
-      <c r="K17" s="32"/>
-      <c r="L17" s="33"/>
+      <c r="J17" s="36"/>
+      <c r="K17" s="36"/>
+      <c r="L17" s="37"/>
     </row>
     <row r="18" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="5"/>
@@ -1066,11 +1076,11 @@
       <c r="F19" s="4"/>
       <c r="G19" s="4"/>
       <c r="H19" s="4"/>
-      <c r="I19" s="28" t="s">
+      <c r="I19" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="J19" s="29"/>
-      <c r="K19" s="30"/>
+      <c r="J19" s="33"/>
+      <c r="K19" s="34"/>
       <c r="L19" s="6"/>
     </row>
     <row r="20" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1092,13 +1102,13 @@
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
-      <c r="E21" s="34" t="s">
+      <c r="E21" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="F21" s="35"/>
-      <c r="G21" s="35"/>
-      <c r="H21" s="35"/>
-      <c r="I21" s="36"/>
+      <c r="F21" s="21"/>
+      <c r="G21" s="21"/>
+      <c r="H21" s="21"/>
+      <c r="I21" s="22"/>
       <c r="J21" s="4"/>
       <c r="K21" s="4"/>
       <c r="L21" s="6"/>
@@ -1122,11 +1132,11 @@
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
-      <c r="E23" s="37" t="s">
+      <c r="E23" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="F23" s="38"/>
-      <c r="G23" s="39"/>
+      <c r="F23" s="26"/>
+      <c r="G23" s="27"/>
       <c r="H23" s="4"/>
       <c r="I23" s="4"/>
       <c r="J23" s="4"/>
@@ -1148,28 +1158,53 @@
       <c r="L24" s="6"/>
     </row>
     <row r="25" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="7"/>
-      <c r="B25" s="8"/>
-      <c r="C25" s="8"/>
-      <c r="D25" s="8"/>
-      <c r="E25" s="37" t="s">
+      <c r="A25" s="5"/>
+      <c r="B25" s="4"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="F25" s="38"/>
-      <c r="G25" s="39"/>
-      <c r="H25" s="8"/>
-      <c r="I25" s="8"/>
-      <c r="J25" s="8"/>
-      <c r="K25" s="8"/>
-      <c r="L25" s="12"/>
+      <c r="F25" s="26"/>
+      <c r="G25" s="27"/>
+      <c r="H25" s="4"/>
+      <c r="I25" s="4"/>
+      <c r="J25" s="4"/>
+      <c r="K25" s="4"/>
+      <c r="L25" s="6"/>
+    </row>
+    <row r="26" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="5"/>
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="11"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="4"/>
+      <c r="H26" s="4"/>
+      <c r="I26" s="4"/>
+      <c r="J26" s="4"/>
+      <c r="K26" s="4"/>
+      <c r="L26" s="6"/>
+    </row>
+    <row r="27" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="7"/>
+      <c r="B27" s="8"/>
+      <c r="C27" s="8"/>
+      <c r="D27" s="8"/>
+      <c r="E27" s="40" t="s">
+        <v>24</v>
+      </c>
+      <c r="F27" s="26"/>
+      <c r="G27" s="26"/>
+      <c r="H27" s="27"/>
+      <c r="I27" s="38"/>
+      <c r="J27" s="38"/>
+      <c r="K27" s="8"/>
+      <c r="L27" s="12"/>
     </row>
   </sheetData>
-  <mergeCells count="13">
-    <mergeCell ref="E21:I21"/>
-    <mergeCell ref="I9:L9"/>
-    <mergeCell ref="I13:L13"/>
-    <mergeCell ref="E23:G23"/>
-    <mergeCell ref="E25:G25"/>
+  <mergeCells count="14">
     <mergeCell ref="D4:I4"/>
     <mergeCell ref="A7:D7"/>
     <mergeCell ref="E8:H8"/>
@@ -1178,6 +1213,12 @@
     <mergeCell ref="J5:L5"/>
     <mergeCell ref="I17:L17"/>
     <mergeCell ref="I11:L11"/>
+    <mergeCell ref="E21:I21"/>
+    <mergeCell ref="I9:L9"/>
+    <mergeCell ref="I13:L13"/>
+    <mergeCell ref="E23:G23"/>
+    <mergeCell ref="E25:G25"/>
+    <mergeCell ref="E27:H27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Re #1 Small comments to Alex project plan in Excel
Former-commit-id: a7bd5e5dcae76b7669696c60dd12c546b813a588
</commit_message>
<xml_diff>
--- a/documentation/design_forV4/WorkPlan.xlsx
+++ b/documentation/design_forV4/WorkPlan.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3750" yWindow="0" windowWidth="21750" windowHeight="10170"/>
+    <workbookView xWindow="4965" yWindow="0" windowWidth="21750" windowHeight="10170"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,40 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
-  <si>
-    <t>W1</t>
-  </si>
-  <si>
-    <t>W2</t>
-  </si>
-  <si>
-    <t>W4</t>
-  </si>
-  <si>
-    <t>W5</t>
-  </si>
-  <si>
-    <t>W6</t>
-  </si>
-  <si>
-    <t>W7</t>
-  </si>
-  <si>
-    <t>W8</t>
-  </si>
-  <si>
-    <t>W9</t>
-  </si>
-  <si>
-    <t>W10</t>
-  </si>
-  <si>
-    <t>W11</t>
-  </si>
-  <si>
-    <t>W12</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
   <si>
     <t>Parallel C++ messaging framework</t>
   </si>
@@ -99,6 +66,60 @@
   </si>
   <si>
     <t xml:space="preserve"> HDF file format</t>
+  </si>
+  <si>
+    <t>Gui for MPI</t>
+  </si>
+  <si>
+    <t>Future cluster wrapper</t>
+  </si>
+  <si>
+    <t>C++ framework optimization</t>
+  </si>
+  <si>
+    <t>mpiexec configurations for non-local clusters</t>
+  </si>
+  <si>
+    <t>Remains on 01/11/2020 in Parallel C++ messagin</t>
+  </si>
+  <si>
+    <t>- minimal requested to state its completed</t>
+  </si>
+  <si>
+    <t>- needed to run it on SCARF or future iDaaaS cluster</t>
+  </si>
+  <si>
+    <t>M1</t>
+  </si>
+  <si>
+    <t>M2</t>
+  </si>
+  <si>
+    <t>M4</t>
+  </si>
+  <si>
+    <t>M5</t>
+  </si>
+  <si>
+    <t>M6</t>
+  </si>
+  <si>
+    <t>M7</t>
+  </si>
+  <si>
+    <t>M8</t>
+  </si>
+  <si>
+    <t>M9</t>
+  </si>
+  <si>
+    <t>M10</t>
+  </si>
+  <si>
+    <t>M11</t>
+  </si>
+  <si>
+    <t>M12</t>
   </si>
 </sst>
 </file>
@@ -396,7 +417,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -418,19 +439,56 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -439,43 +497,7 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -763,53 +785,53 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L27"/>
+  <dimension ref="A1:U27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="Q7" sqref="Q7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="16" t="s">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="B1" s="17" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="C1" s="17" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="D1" s="17" t="s">
-        <v>2</v>
+        <v>23</v>
       </c>
       <c r="E1" s="17" t="s">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="F1" s="17" t="s">
-        <v>4</v>
+        <v>25</v>
       </c>
       <c r="G1" s="17" t="s">
-        <v>5</v>
+        <v>26</v>
       </c>
       <c r="H1" s="17" t="s">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="I1" s="17" t="s">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="J1" s="17" t="s">
-        <v>8</v>
+        <v>29</v>
       </c>
       <c r="K1" s="17" t="s">
-        <v>9</v>
+        <v>30</v>
       </c>
       <c r="L1" s="18" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="19"/>
       <c r="B2" s="13"/>
       <c r="C2" s="13"/>
@@ -822,10 +844,13 @@
       <c r="J2" s="11"/>
       <c r="K2" s="13"/>
       <c r="L2" s="20"/>
-    </row>
-    <row r="3" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="9"/>
@@ -838,24 +863,33 @@
       <c r="J3" s="3"/>
       <c r="K3" s="4"/>
       <c r="L3" s="6"/>
-    </row>
-    <row r="4" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P3" t="s">
+        <v>17</v>
+      </c>
+      <c r="U3" s="41" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
-      <c r="D4" s="28" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" s="29"/>
-      <c r="F4" s="29"/>
-      <c r="G4" s="29"/>
-      <c r="H4" s="29"/>
-      <c r="I4" s="30"/>
+      <c r="D4" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="23"/>
+      <c r="H4" s="23"/>
+      <c r="I4" s="24"/>
       <c r="J4" s="4"/>
       <c r="K4" s="4"/>
       <c r="L4" s="6"/>
-    </row>
-    <row r="5" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -865,13 +899,19 @@
       <c r="G5" s="13"/>
       <c r="H5" s="13"/>
       <c r="I5" s="11"/>
-      <c r="J5" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="K5" s="29"/>
-      <c r="L5" s="30"/>
-    </row>
-    <row r="6" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J5" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="K5" s="23"/>
+      <c r="L5" s="24"/>
+      <c r="P5" t="s">
+        <v>15</v>
+      </c>
+      <c r="U5" s="41" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
@@ -884,14 +924,17 @@
       <c r="J6" s="4"/>
       <c r="K6" s="4"/>
       <c r="L6" s="6"/>
-    </row>
-    <row r="7" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="31" t="s">
+      <c r="P6" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="24"/>
-      <c r="C7" s="24"/>
-      <c r="D7" s="24"/>
+    </row>
+    <row r="7" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="26"/>
+      <c r="C7" s="26"/>
+      <c r="D7" s="26"/>
       <c r="E7" s="3"/>
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
@@ -901,23 +944,23 @@
       <c r="K7" s="4"/>
       <c r="L7" s="6"/>
     </row>
-    <row r="8" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
-      <c r="E8" s="23" t="s">
-        <v>15</v>
-      </c>
-      <c r="F8" s="24"/>
-      <c r="G8" s="24"/>
-      <c r="H8" s="24"/>
+      <c r="E8" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="F8" s="26"/>
+      <c r="G8" s="26"/>
+      <c r="H8" s="26"/>
       <c r="I8" s="10"/>
       <c r="J8" s="4"/>
       <c r="K8" s="4"/>
       <c r="L8" s="6"/>
     </row>
-    <row r="9" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
@@ -926,14 +969,14 @@
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>
-      <c r="I9" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="J9" s="24"/>
-      <c r="K9" s="24"/>
-      <c r="L9" s="25"/>
-    </row>
-    <row r="10" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I9" s="27" t="s">
+        <v>2</v>
+      </c>
+      <c r="J9" s="26"/>
+      <c r="K9" s="26"/>
+      <c r="L9" s="28"/>
+    </row>
+    <row r="10" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -947,7 +990,7 @@
       <c r="K10" s="4"/>
       <c r="L10" s="6"/>
     </row>
-    <row r="11" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
@@ -956,14 +999,14 @@
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
-      <c r="I11" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="J11" s="24"/>
-      <c r="K11" s="24"/>
-      <c r="L11" s="25"/>
-    </row>
-    <row r="12" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I11" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="J11" s="26"/>
+      <c r="K11" s="26"/>
+      <c r="L11" s="28"/>
+    </row>
+    <row r="12" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
@@ -977,7 +1020,7 @@
       <c r="K12" s="4"/>
       <c r="L12" s="6"/>
     </row>
-    <row r="13" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="5"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
@@ -986,14 +1029,14 @@
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
-      <c r="I13" s="23" t="s">
-        <v>18</v>
-      </c>
-      <c r="J13" s="24"/>
-      <c r="K13" s="24"/>
-      <c r="L13" s="25"/>
-    </row>
-    <row r="14" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I13" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="J13" s="26"/>
+      <c r="K13" s="26"/>
+      <c r="L13" s="28"/>
+    </row>
+    <row r="14" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="5"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
@@ -1007,7 +1050,7 @@
       <c r="K14" s="4"/>
       <c r="L14" s="6"/>
     </row>
-    <row r="15" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="5"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
@@ -1016,14 +1059,14 @@
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
-      <c r="I15" s="23" t="s">
-        <v>20</v>
-      </c>
-      <c r="J15" s="24"/>
-      <c r="K15" s="24"/>
-      <c r="L15" s="25"/>
-    </row>
-    <row r="16" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I15" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="J15" s="26"/>
+      <c r="K15" s="26"/>
+      <c r="L15" s="28"/>
+    </row>
+    <row r="16" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="5"/>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
@@ -1046,12 +1089,12 @@
       <c r="F17" s="4"/>
       <c r="G17" s="4"/>
       <c r="H17" s="4"/>
-      <c r="I17" s="35" t="s">
-        <v>12</v>
-      </c>
-      <c r="J17" s="36"/>
-      <c r="K17" s="36"/>
-      <c r="L17" s="37"/>
+      <c r="I17" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="J17" s="33"/>
+      <c r="K17" s="33"/>
+      <c r="L17" s="34"/>
     </row>
     <row r="18" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="5"/>
@@ -1076,11 +1119,11 @@
       <c r="F19" s="4"/>
       <c r="G19" s="4"/>
       <c r="H19" s="4"/>
-      <c r="I19" s="32" t="s">
-        <v>19</v>
-      </c>
-      <c r="J19" s="33"/>
-      <c r="K19" s="34"/>
+      <c r="I19" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="J19" s="30"/>
+      <c r="K19" s="31"/>
       <c r="L19" s="6"/>
     </row>
     <row r="20" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1102,13 +1145,13 @@
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
-      <c r="E21" s="39" t="s">
-        <v>23</v>
-      </c>
-      <c r="F21" s="21"/>
-      <c r="G21" s="21"/>
-      <c r="H21" s="21"/>
-      <c r="I21" s="22"/>
+      <c r="E21" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="F21" s="36"/>
+      <c r="G21" s="36"/>
+      <c r="H21" s="36"/>
+      <c r="I21" s="37"/>
       <c r="J21" s="4"/>
       <c r="K21" s="4"/>
       <c r="L21" s="6"/>
@@ -1132,11 +1175,11 @@
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
-      <c r="E23" s="40" t="s">
-        <v>19</v>
-      </c>
-      <c r="F23" s="26"/>
-      <c r="G23" s="27"/>
+      <c r="E23" s="38" t="s">
+        <v>8</v>
+      </c>
+      <c r="F23" s="39"/>
+      <c r="G23" s="40"/>
       <c r="H23" s="4"/>
       <c r="I23" s="4"/>
       <c r="J23" s="4"/>
@@ -1162,11 +1205,11 @@
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
-      <c r="E25" s="40" t="s">
-        <v>22</v>
-      </c>
-      <c r="F25" s="26"/>
-      <c r="G25" s="27"/>
+      <c r="E25" s="38" t="s">
+        <v>11</v>
+      </c>
+      <c r="F25" s="39"/>
+      <c r="G25" s="40"/>
       <c r="H25" s="4"/>
       <c r="I25" s="4"/>
       <c r="J25" s="4"/>
@@ -1192,19 +1235,25 @@
       <c r="B27" s="8"/>
       <c r="C27" s="8"/>
       <c r="D27" s="8"/>
-      <c r="E27" s="40" t="s">
-        <v>24</v>
-      </c>
-      <c r="F27" s="26"/>
-      <c r="G27" s="26"/>
-      <c r="H27" s="27"/>
-      <c r="I27" s="38"/>
-      <c r="J27" s="38"/>
+      <c r="E27" s="38" t="s">
+        <v>13</v>
+      </c>
+      <c r="F27" s="39"/>
+      <c r="G27" s="39"/>
+      <c r="H27" s="40"/>
+      <c r="I27" s="21"/>
+      <c r="J27" s="21"/>
       <c r="K27" s="8"/>
       <c r="L27" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="E27:H27"/>
+    <mergeCell ref="E21:I21"/>
+    <mergeCell ref="I9:L9"/>
+    <mergeCell ref="I13:L13"/>
+    <mergeCell ref="E23:G23"/>
+    <mergeCell ref="E25:G25"/>
     <mergeCell ref="D4:I4"/>
     <mergeCell ref="A7:D7"/>
     <mergeCell ref="E8:H8"/>
@@ -1213,12 +1262,6 @@
     <mergeCell ref="J5:L5"/>
     <mergeCell ref="I17:L17"/>
     <mergeCell ref="I11:L11"/>
-    <mergeCell ref="E21:I21"/>
-    <mergeCell ref="I9:L9"/>
-    <mergeCell ref="I13:L13"/>
-    <mergeCell ref="E23:G23"/>
-    <mergeCell ref="E25:G25"/>
-    <mergeCell ref="E27:H27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>